<commit_message>
typo in DeNaZin track file; fixed jQuery selection for rows in phpDynamicTbles.js
</commit_message>
<xml_diff>
--- a/data/HikeDB.xlsx
+++ b/data/HikeDB.xlsx
@@ -2655,9 +2655,6 @@
     <t>De_Na_Zin.GPX</t>
   </si>
   <si>
-    <t>De_Na-Zin.json</t>
-  </si>
-  <si>
     <t>https://www.flickr.com/photos/139088815@N08/albums/72157674420137292</t>
   </si>
   <si>
@@ -2851,6 +2848,9 @@
   </si>
   <si>
     <t>Use markerID for a Visitor Center hike as if standalone: eg single, "normal"; multiple "cluster"</t>
+  </si>
+  <si>
+    <t>De_Na_Zin.json</t>
   </si>
 </sst>
 </file>
@@ -3376,10 +3376,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC323"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="B116" sqref="B116"/>
+      <selection pane="bottomLeft" activeCell="S96" sqref="S96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3446,10 +3446,10 @@
         <v>38</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>3</v>
@@ -3518,7 +3518,7 @@
         <v>21</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="3" spans="1:29">
@@ -3564,7 +3564,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C4" t="s">
         <v>54</v>
@@ -3602,7 +3602,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="C5" t="s">
         <v>59</v>
@@ -3637,7 +3637,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C6" t="s">
         <v>63</v>
@@ -4051,7 +4051,7 @@
         <v>98</v>
       </c>
       <c r="AC12" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="13" spans="1:29">
@@ -4116,7 +4116,7 @@
         <v>105</v>
       </c>
       <c r="AC13" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="14" spans="1:29">
@@ -4193,7 +4193,7 @@
         <v>133</v>
       </c>
       <c r="AC14" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="15" spans="1:29">
@@ -4270,7 +4270,7 @@
         <v>141</v>
       </c>
       <c r="AC15" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="16" spans="1:29">
@@ -4347,7 +4347,7 @@
         <v>152</v>
       </c>
       <c r="AC16" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="17" spans="1:29">
@@ -4424,7 +4424,7 @@
         <v>158</v>
       </c>
       <c r="AC17" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="18" spans="1:29">
@@ -4489,7 +4489,7 @@
         <v>165</v>
       </c>
       <c r="AC18" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="19" spans="1:29">
@@ -4554,7 +4554,7 @@
         <v>168</v>
       </c>
       <c r="AC19" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="20" spans="1:29">
@@ -4619,7 +4619,7 @@
         <v>171</v>
       </c>
       <c r="AC20" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="21" spans="1:29">
@@ -4699,7 +4699,7 @@
         <v>186</v>
       </c>
       <c r="AC21" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="22" spans="1:29">
@@ -4773,7 +4773,7 @@
         <v>194</v>
       </c>
       <c r="AC22" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="23" spans="1:29">
@@ -4850,7 +4850,7 @@
         <v>203</v>
       </c>
       <c r="AC23" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="24" spans="1:29">
@@ -4927,7 +4927,7 @@
         <v>217</v>
       </c>
       <c r="AC24" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="25" spans="1:29">
@@ -5004,7 +5004,7 @@
         <v>225</v>
       </c>
       <c r="AC25" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="26" spans="1:29">
@@ -5081,7 +5081,7 @@
         <v>235</v>
       </c>
       <c r="AC26" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="27" spans="1:29">
@@ -5155,7 +5155,7 @@
         <v>245</v>
       </c>
       <c r="AC27" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="28" spans="1:29">
@@ -5232,7 +5232,7 @@
         <v>255</v>
       </c>
       <c r="AC28" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="29" spans="1:29">
@@ -5309,7 +5309,7 @@
         <v>267</v>
       </c>
       <c r="AC29" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="30" spans="1:29">
@@ -5386,7 +5386,7 @@
         <v>276</v>
       </c>
       <c r="AC30" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="31" spans="1:29">
@@ -5464,7 +5464,7 @@
         <v>336</v>
       </c>
       <c r="AC31" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="32" spans="1:29">
@@ -5541,7 +5541,7 @@
         <v>851</v>
       </c>
       <c r="AC32" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="33" spans="1:28">
@@ -9666,7 +9666,7 @@
         <v>877</v>
       </c>
       <c r="S95" t="s">
-        <v>878</v>
+        <v>943</v>
       </c>
       <c r="T95" s="5">
         <v>36.311774999999997</v>
@@ -9675,16 +9675,16 @@
         <v>-108.00259440000001</v>
       </c>
       <c r="X95" t="s">
+        <v>878</v>
+      </c>
+      <c r="Z95" t="s">
         <v>879</v>
-      </c>
-      <c r="Z95" t="s">
-        <v>880</v>
       </c>
       <c r="AA95" t="s">
         <v>45</v>
       </c>
       <c r="AB95" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="96" spans="1:28">
@@ -9692,10 +9692,10 @@
         <v>97</v>
       </c>
       <c r="B96" t="s">
+        <v>881</v>
+      </c>
+      <c r="C96" t="s">
         <v>882</v>
-      </c>
-      <c r="C96" t="s">
-        <v>883</v>
       </c>
       <c r="D96" t="s">
         <v>42</v>
@@ -9725,19 +9725,19 @@
         <v>35</v>
       </c>
       <c r="O96" t="s">
+        <v>883</v>
+      </c>
+      <c r="P96" t="s">
         <v>884</v>
       </c>
-      <c r="P96" t="s">
+      <c r="Q96" t="s">
         <v>885</v>
       </c>
-      <c r="Q96" t="s">
+      <c r="R96" t="s">
         <v>886</v>
       </c>
-      <c r="R96" t="s">
+      <c r="S96" t="s">
         <v>887</v>
-      </c>
-      <c r="S96" t="s">
-        <v>888</v>
       </c>
       <c r="T96" s="5">
         <v>36.241438899999999</v>
@@ -9746,16 +9746,16 @@
         <v>-108.2632335</v>
       </c>
       <c r="X96" t="s">
+        <v>888</v>
+      </c>
+      <c r="Z96" t="s">
         <v>889</v>
-      </c>
-      <c r="Z96" t="s">
-        <v>890</v>
       </c>
       <c r="AA96" t="s">
         <v>45</v>
       </c>
       <c r="AB96" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="97" spans="1:28">
@@ -9763,7 +9763,7 @@
         <v>98</v>
       </c>
       <c r="B97" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="C97" t="s">
         <v>63</v>
@@ -9787,7 +9787,7 @@
         <v>122</v>
       </c>
       <c r="L97" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="M97" t="s">
         <v>124</v>
@@ -9796,19 +9796,19 @@
         <v>36</v>
       </c>
       <c r="O97" t="s">
+        <v>893</v>
+      </c>
+      <c r="P97" t="s">
         <v>894</v>
       </c>
-      <c r="P97" t="s">
+      <c r="Q97" t="s">
         <v>895</v>
       </c>
-      <c r="Q97" t="s">
+      <c r="R97" t="s">
         <v>896</v>
       </c>
-      <c r="R97" t="s">
+      <c r="S97" t="s">
         <v>897</v>
-      </c>
-      <c r="S97" t="s">
-        <v>898</v>
       </c>
       <c r="T97" s="5">
         <v>35.222724999999997</v>
@@ -9817,16 +9817,16 @@
         <v>-106.48348</v>
       </c>
       <c r="X97" t="s">
+        <v>905</v>
+      </c>
+      <c r="Z97" t="s">
         <v>906</v>
-      </c>
-      <c r="Z97" t="s">
-        <v>907</v>
       </c>
       <c r="AA97" t="s">
         <v>45</v>
       </c>
       <c r="AB97" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="98" spans="1:28">
@@ -9834,7 +9834,7 @@
         <v>99</v>
       </c>
       <c r="B98" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="C98" t="s">
         <v>63</v>
@@ -9858,7 +9858,7 @@
         <v>68</v>
       </c>
       <c r="L98" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="M98" t="s">
         <v>634</v>
@@ -9867,16 +9867,16 @@
         <v>35</v>
       </c>
       <c r="O98" t="s">
+        <v>901</v>
+      </c>
+      <c r="P98" t="s">
         <v>902</v>
       </c>
-      <c r="P98" t="s">
+      <c r="R98" t="s">
         <v>903</v>
       </c>
-      <c r="R98" t="s">
+      <c r="S98" t="s">
         <v>904</v>
-      </c>
-      <c r="S98" t="s">
-        <v>905</v>
       </c>
       <c r="T98" s="5">
         <v>35.130690000000001</v>
@@ -9885,16 +9885,16 @@
         <v>-106.684523</v>
       </c>
       <c r="X98" t="s">
+        <v>907</v>
+      </c>
+      <c r="Z98" t="s">
         <v>908</v>
-      </c>
-      <c r="Z98" t="s">
-        <v>909</v>
       </c>
       <c r="AA98" t="s">
         <v>45</v>
       </c>
       <c r="AB98" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="99" spans="1:28">
@@ -9902,7 +9902,7 @@
         <v>100</v>
       </c>
       <c r="B99" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C99" t="s">
         <v>345</v>
@@ -9914,10 +9914,10 @@
         <v>24</v>
       </c>
       <c r="H99" s="7" t="s">
+        <v>911</v>
+      </c>
+      <c r="I99" s="7" t="s">
         <v>912</v>
-      </c>
-      <c r="I99" s="7" t="s">
-        <v>913</v>
       </c>
       <c r="J99" t="s">
         <v>29</v>
@@ -9935,19 +9935,19 @@
         <v>35</v>
       </c>
       <c r="O99" t="s">
+        <v>913</v>
+      </c>
+      <c r="P99" t="s">
         <v>914</v>
       </c>
-      <c r="P99" t="s">
+      <c r="Q99" t="s">
         <v>915</v>
       </c>
-      <c r="Q99" t="s">
+      <c r="R99" t="s">
         <v>916</v>
       </c>
-      <c r="R99" t="s">
+      <c r="S99" t="s">
         <v>917</v>
-      </c>
-      <c r="S99" t="s">
-        <v>918</v>
       </c>
       <c r="T99" s="5">
         <v>35.450367</v>
@@ -9956,16 +9956,16 @@
         <v>-106.13902299999999</v>
       </c>
       <c r="X99" t="s">
+        <v>918</v>
+      </c>
+      <c r="Z99" t="s">
         <v>919</v>
-      </c>
-      <c r="Z99" t="s">
-        <v>920</v>
       </c>
       <c r="AA99" t="s">
         <v>45</v>
       </c>
       <c r="AB99" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="100" spans="1:28">
@@ -9973,7 +9973,7 @@
         <v>101</v>
       </c>
       <c r="B100" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="C100" t="s">
         <v>385</v>
@@ -10056,7 +10056,7 @@
         <v>111</v>
       </c>
       <c r="B110" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="111" spans="1:28">
@@ -10067,7 +10067,7 @@
         <v>1</v>
       </c>
       <c r="C111" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="112" spans="1:28">
@@ -10078,7 +10078,7 @@
         <v>2</v>
       </c>
       <c r="C112" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -10089,7 +10089,7 @@
         <v>3</v>
       </c>
       <c r="C113" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -10100,7 +10100,7 @@
         <v>4</v>
       </c>
       <c r="C114" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -10111,7 +10111,7 @@
         <v>5</v>
       </c>
       <c r="C115" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="116" spans="1:3">

</xml_diff>